<commit_message>
run it flush & pair
</commit_message>
<xml_diff>
--- a/poker/hold_em_worksheet.xlsx
+++ b/poker/hold_em_worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eastmanchem-my.sharepoint.com/personal/u773253_emn_com/Documents/MJ/Coding/card_games/poker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{1D3D71A7-F436-4DD9-BFB8-33B077D07F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4641EB92-5EE1-47BB-913A-148A39C8B267}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{1D3D71A7-F436-4DD9-BFB8-33B077D07F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA15EE73-CBA3-445C-8598-B500195F0425}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C1F3730-037F-48F6-96B0-BBBEA2325824}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{8C1F3730-037F-48F6-96B0-BBBEA2325824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -494,19 +494,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R2:U14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -582,7 +582,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K3">
         <v>3</v>
       </c>
@@ -606,7 +606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K4">
         <v>4</v>
       </c>
@@ -630,7 +630,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>16</v>
       </c>
@@ -657,7 +657,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -687,7 +687,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -718,13 +718,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <f>B2</f>
-        <v>24</v>
+        <f>9+13</f>
+        <v>22</v>
       </c>
       <c r="K8">
         <v>8</v>
@@ -749,7 +749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -776,7 +776,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -807,13 +807,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11">
-        <f>C2</f>
-        <v>25</v>
+        <f>10+13</f>
+        <v>23</v>
       </c>
       <c r="K11" t="s">
         <v>5</v>
@@ -838,7 +838,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -865,7 +865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -895,7 +895,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -928,7 +928,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -939,7 +939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -950,7 +950,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -958,7 +958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -972,7 +972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>
@@ -986,12 +986,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>14</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>15</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>16</v>
       </c>
@@ -1042,12 +1042,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>18</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1066,162 +1066,162 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>51</v>
       </c>

</xml_diff>